<commit_message>
add Supp Table S4
</commit_message>
<xml_diff>
--- a/figures_tables/supp/SupplementaryTable.xlsx
+++ b/figures_tables/supp/SupplementaryTable.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liaoc/Documents/Source_code_for_SCFA_dynamics_project/figures_tables/supp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952EC68C-0CE0-4C4B-BDEF-4A7B0BF7DF85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F6D96-21D0-4841-84A5-96B072A485EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38320" yWindow="1380" windowWidth="30940" windowHeight="16900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42900" yWindow="1400" windowWidth="30940" windowHeight="16900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="2" r:id="rId1"/>
     <sheet name="Table S2" sheetId="4" r:id="rId2"/>
     <sheet name="Table S3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table S4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="162">
   <si>
     <t>Cellulose</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -283,18 +284,12 @@
     <t>Butyrate</t>
   </si>
   <si>
-    <t>&lt;0.001</t>
-  </si>
-  <si>
     <t>Propionate</t>
   </si>
   <si>
     <t>Acetate</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>Shanghai</t>
   </si>
   <si>
@@ -305,70 +300,6 @@
   </si>
   <si>
     <t>Beijing</t>
-  </si>
-  <si>
-    <t>1.97 (±1.62)</t>
-  </si>
-  <si>
-    <t>3.18 (±1.80)</t>
-  </si>
-  <si>
-    <t>0.84 (±0.19)</t>
-  </si>
-  <si>
-    <t>0.63 (±0.13)</t>
-  </si>
-  <si>
-    <t>0.45 (±0.15)</t>
-  </si>
-  <si>
-    <t>1.00 (±0.35)</t>
-  </si>
-  <si>
-    <t>0.42 (±0.22)</t>
-  </si>
-  <si>
-    <t>7.83 (±0.52)</t>
-  </si>
-  <si>
-    <t>0.35 (±0.17)</t>
-  </si>
-  <si>
-    <t>0.88 (±0.20)</t>
-  </si>
-  <si>
-    <t>0.46 (±0.18)</t>
-  </si>
-  <si>
-    <t>0.38 (±0.16)</t>
-  </si>
-  <si>
-    <t>0.56 (±0.31)</t>
-  </si>
-  <si>
-    <t>0.93 (±0.43)</t>
-  </si>
-  <si>
-    <t>0.47 (±0.18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.39 (±0.11)</t>
-  </si>
-  <si>
-    <t>0.13 (±0.14)</t>
-  </si>
-  <si>
-    <t>0.75 (±0.36)</t>
-  </si>
-  <si>
-    <t>0.10 (±0.15)</t>
-  </si>
-  <si>
-    <t>1.64 (±1.68)</t>
-  </si>
-  <si>
-    <t>Table S1. Ingredients and analyzed chemical composition of the four experimental diets.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -524,6 +455,263 @@
   <si>
     <t>Table S2. Damping ratio of dynamic responses of gut microbiota and short-chain fatty acids (SCFAs) to inulin treatment</t>
   </si>
+  <si>
+    <t>1.00, 1.00, 1.00, 1.42, 2.49</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.00, 7379.43</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.00, 1.00</t>
+  </si>
+  <si>
+    <t>1.00, 1.04, 19.57, 37.02, 3965.86</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.00, 2.10, 8187.40</t>
+  </si>
+  <si>
+    <t>1.00, 1.70, 6.09, 4816.12</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.00, 1.00, 1.92</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.02, 1.20, 1.38</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 2.14, 4.48</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.07, 3.11</t>
+  </si>
+  <si>
+    <t>1.02, 85.81, 5417.51, 8178.45, 15661.28</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.00, 1.00, 1.00</t>
+  </si>
+  <si>
+    <t>1.00, 1.14, 1.27, 1.39</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.00, 1.38, 1.76</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.00, 1.00, 3.80</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.80, 3.38</t>
+  </si>
+  <si>
+    <t>1.00, 1.00, 1.00, 1.00, 1.73</t>
+  </si>
+  <si>
+    <t>Note: the values of damping ratio are reported in a per-mouse basis.</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Pi</t>
+  </si>
+  <si>
+    <t>Pr</t>
+  </si>
+  <si>
+    <t>Lachnospiraceae bacterium 28-4</t>
+  </si>
+  <si>
+    <t>Un. Family XIII AD3011 group</t>
+  </si>
+  <si>
+    <t>Un. Rikenella</t>
+  </si>
+  <si>
+    <t>Un. Negativibacillus</t>
+  </si>
+  <si>
+    <t>Un. Parabacteroides</t>
+  </si>
+  <si>
+    <t>Table S1. Ingredients and analyzed chemical composition of the four experimental diets.</t>
+  </si>
+  <si>
+    <t>Un. Anaerovorax</t>
+  </si>
+  <si>
+    <t>Un. [Eubacterium] xylanophilum group</t>
+  </si>
+  <si>
+    <t>Un. UBA1819</t>
+  </si>
+  <si>
+    <t>Un. Candidatus-Saccharimonas</t>
+  </si>
+  <si>
+    <t>Un. Rikenellaceae RC9 gut group</t>
+  </si>
+  <si>
+    <t>Desulfovibrio fairfieldensis</t>
+  </si>
+  <si>
+    <t>Un. [Eubacterium] nodatum group</t>
+  </si>
+  <si>
+    <t>Clostridiales bacterium CIEAF 012</t>
+  </si>
+  <si>
+    <t>Un. Clostridia vadinBB60 group</t>
+  </si>
+  <si>
+    <t>Un. Christensenellaceae</t>
+  </si>
+  <si>
+    <t>Bacteroides nordii</t>
+  </si>
+  <si>
+    <t>Un. Blautia</t>
+  </si>
+  <si>
+    <t>Un. Alistipes</t>
+  </si>
+  <si>
+    <t>Un. Clostridium sensu stricto 1</t>
+  </si>
+  <si>
+    <t>Un. Odoribacter</t>
+  </si>
+  <si>
+    <t>Un. Ruminococcaceae</t>
+  </si>
+  <si>
+    <t>Un. Colidextribacter</t>
+  </si>
+  <si>
+    <t>Un. Tuzzerella</t>
+  </si>
+  <si>
+    <t>Un. NK4A214 group</t>
+  </si>
+  <si>
+    <t>Un. Desulfovibrio</t>
+  </si>
+  <si>
+    <t>[Clostridium] leptum</t>
+  </si>
+  <si>
+    <t>Un. Bacteroides</t>
+  </si>
+  <si>
+    <t>Un. Alloprevotella</t>
+  </si>
+  <si>
+    <t>Un. Lachnospiraceae NK4A136 group</t>
+  </si>
+  <si>
+    <t>Mouse-gut-metagenome</t>
+  </si>
+  <si>
+    <t>Alistipes shahii</t>
+  </si>
+  <si>
+    <t>Bacteroides acidifaciens</t>
+  </si>
+  <si>
+    <t>Bacteroides caecimuris</t>
+  </si>
+  <si>
+    <t>Un. Faecalibaculum</t>
+  </si>
+  <si>
+    <t>Christensenella sp. Marseille-P2437</t>
+  </si>
+  <si>
+    <t>Un. Prevotellaceae UCG-001</t>
+  </si>
+  <si>
+    <t>Un. Muribaculaceae</t>
+  </si>
+  <si>
+    <t>Un. Bacteria</t>
+  </si>
+  <si>
+    <t>Un. Parasutterella</t>
+  </si>
+  <si>
+    <t>Un. Gastranaerophilales</t>
+  </si>
+  <si>
+    <t>Un. Muribaculum</t>
+  </si>
+  <si>
+    <t>Akkermansia muciniphila</t>
+  </si>
+  <si>
+    <t>Bifidobacterium choerinum</t>
+  </si>
+  <si>
+    <t>Un. Tannerellaceae</t>
+  </si>
+  <si>
+    <t>Bacteroides uniformis</t>
+  </si>
+  <si>
+    <t>Un. Coriobacteriaceae UCG-002</t>
+  </si>
+  <si>
+    <t>Un. Frisingicoccus</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <r>
+      <t>Table S4. Bacterial species with significant individualized responses (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">positive response in red </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>negative response in blue</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) to inulin treatment. FC: ratio of averaged area under the absolute abundance curve between inulin and cellulose group. Pr: P-value for significance test of responsiveness (compared between inulin and cellulose group). Pi: P-value for significance test of individuality (compared across different vendors). We listed all species that have Pr&lt;0.05 and Pi&lt;0.05 below.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -533,7 +721,7 @@
     <numFmt numFmtId="164" formatCode="[DBNum1][$-804]General"/>
     <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -666,20 +854,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -752,7 +966,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -850,9 +1064,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -874,7 +1085,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
@@ -897,6 +1108,27 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1193,7 +1425,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1203,40 +1435,40 @@
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="46" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="47"/>
+      <c r="F2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="46"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" spans="1:14" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="42" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1848,7 +2080,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -1859,7 +2091,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -2181,154 +2413,148 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B52425-C74A-49AA-B81C-288F4CED1F6B}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="35" customWidth="1"/>
-    <col min="2" max="6" width="20.83203125" style="35" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="35" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="35" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" style="35" customWidth="1"/>
-    <col min="10" max="10" width="19.5" style="35" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" style="35" customWidth="1"/>
-    <col min="12" max="12" width="9.5" style="35" customWidth="1"/>
-    <col min="13" max="16384" width="13.1640625" style="35"/>
+    <col min="1" max="1" width="15.5" style="34" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="35.5" style="34" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="34" customWidth="1"/>
+    <col min="7" max="7" width="18.5" style="34" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="34" customWidth="1"/>
+    <col min="9" max="9" width="19.5" style="34" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" style="34" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="34" customWidth="1"/>
+    <col min="12" max="16384" width="13.1640625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-    </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36"/>
+        <v>90</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="35"/>
       <c r="B2" s="32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="37">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="37" t="s">
+      <c r="B3" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="B4" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="37">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="B5" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="37">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="B6" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="38">
-        <v>0.85</v>
-      </c>
+      <c r="B7" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2338,9 +2564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BB7F8A-EE5F-4C2C-B960-534A0B649BA2}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2351,25 +2575,25 @@
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="45" t="s">
+    <row r="2" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2392,7 +2616,7 @@
         <v>43</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2448,7 +2672,7 @@
         <v>57</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2463,8 +2687,8 @@
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="39" t="s">
-        <v>100</v>
+      <c r="B10" s="38" t="s">
+        <v>77</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>56</v>
@@ -2477,8 +2701,8 @@
       <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>102</v>
+      <c r="B11" s="38" t="s">
+        <v>79</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>46</v>
@@ -2491,14 +2715,14 @@
       <c r="A12" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="40" t="s">
-        <v>103</v>
+      <c r="B12" s="39" t="s">
+        <v>80</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2543,52 +2767,52 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2596,4 +2820,709 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E999810-1AF7-BB4F-97F1-E2A8A2831BA7}">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="31" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31" style="53"/>
+    <col min="2" max="2" width="8.6640625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="53" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="53" customWidth="1"/>
+    <col min="5" max="16384" width="31" style="53"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="115" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="51">
+        <v>0.123062434</v>
+      </c>
+      <c r="C3" s="51">
+        <v>1.5523403999999999E-2</v>
+      </c>
+      <c r="D3" s="51">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="51">
+        <v>0.13617238199999901</v>
+      </c>
+      <c r="C4" s="51">
+        <v>9.4999999999999897E-5</v>
+      </c>
+      <c r="D4" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="51">
+        <v>0.163568832</v>
+      </c>
+      <c r="C5" s="51">
+        <v>6.0799999999999899E-3</v>
+      </c>
+      <c r="D5" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="51">
+        <v>0.18519186699999901</v>
+      </c>
+      <c r="C6" s="51">
+        <v>1.07293999999999E-4</v>
+      </c>
+      <c r="D6" s="51">
+        <v>9.6500000000000008E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="51">
+        <v>0.25741119400000001</v>
+      </c>
+      <c r="C7" s="51">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D7" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="51">
+        <v>0.29381153700000001</v>
+      </c>
+      <c r="C8" s="51">
+        <v>1.4539129999999901E-3</v>
+      </c>
+      <c r="D8" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="51">
+        <v>0.30391195500000001</v>
+      </c>
+      <c r="C9" s="51">
+        <v>2.1714289999999999E-3</v>
+      </c>
+      <c r="D9" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="51">
+        <v>0.342614009</v>
+      </c>
+      <c r="C10" s="51">
+        <v>3.3295237999999998E-2</v>
+      </c>
+      <c r="D10" s="51">
+        <v>2.7794289999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="51">
+        <v>0.35105807299999903</v>
+      </c>
+      <c r="C11" s="51">
+        <v>2.5333333E-2</v>
+      </c>
+      <c r="D11" s="51">
+        <v>6.843979E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="51">
+        <v>0.39149551599999999</v>
+      </c>
+      <c r="C12" s="51">
+        <v>8.1560980000000005E-3</v>
+      </c>
+      <c r="D12" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="51">
+        <v>0.397484642</v>
+      </c>
+      <c r="C13" s="51">
+        <v>1.1054545000000001E-2</v>
+      </c>
+      <c r="D13" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="51">
+        <v>0.40328616699999997</v>
+      </c>
+      <c r="C14" s="51">
+        <v>8.6857140000000006E-3</v>
+      </c>
+      <c r="D14" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="51">
+        <v>0.433470048</v>
+      </c>
+      <c r="C15" s="51">
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="D15" s="51">
+        <v>5.9607799999999999E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="51">
+        <v>0.45021419699999998</v>
+      </c>
+      <c r="C16" s="51">
+        <v>2.3969231000000001E-2</v>
+      </c>
+      <c r="D16" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="51">
+        <v>0.469705655</v>
+      </c>
+      <c r="C17" s="51">
+        <v>2.1955599999999901E-4</v>
+      </c>
+      <c r="D17" s="51">
+        <v>7.5099999999999901E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="51">
+        <v>0.47023225799999901</v>
+      </c>
+      <c r="C18" s="51">
+        <v>1.5523403999999999E-2</v>
+      </c>
+      <c r="D18" s="51">
+        <v>2.6358379999999902E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="51">
+        <v>0.50909777499999997</v>
+      </c>
+      <c r="C19" s="51">
+        <v>2.3969231000000001E-2</v>
+      </c>
+      <c r="D19" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="51">
+        <v>0.53361474600000003</v>
+      </c>
+      <c r="C20" s="51">
+        <v>6.2358969999999998E-3</v>
+      </c>
+      <c r="D20" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="51">
+        <v>0.53733575299999903</v>
+      </c>
+      <c r="C21" s="51">
+        <v>4.2375757999999999E-2</v>
+      </c>
+      <c r="D21" s="51">
+        <v>1.06047E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="51">
+        <v>0.57189861099999995</v>
+      </c>
+      <c r="C22" s="51">
+        <v>6.2358969999999998E-3</v>
+      </c>
+      <c r="D22" s="51">
+        <v>1.2999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="51">
+        <v>0.582515805</v>
+      </c>
+      <c r="C23" s="51">
+        <v>6.0800000000000001E-5</v>
+      </c>
+      <c r="D23" s="51">
+        <v>9.6500000000000008E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="51">
+        <v>0.80738405400000002</v>
+      </c>
+      <c r="C24" s="51">
+        <v>2.8228571000000001E-2</v>
+      </c>
+      <c r="D24" s="51">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="51">
+        <v>0.88909589200000005</v>
+      </c>
+      <c r="C25" s="51">
+        <v>4.1325000000000001E-2</v>
+      </c>
+      <c r="D25" s="51">
+        <v>2.1714289999999999E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="52">
+        <v>1.0174382850000001</v>
+      </c>
+      <c r="C26" s="52">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="D26" s="52">
+        <v>1.4139529999999999E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="52">
+        <v>1.1039773239999999</v>
+      </c>
+      <c r="C27" s="52">
+        <v>5.7904799999999998E-4</v>
+      </c>
+      <c r="D27" s="52">
+        <v>5.2583780000000002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="52">
+        <v>1.8546868519999999</v>
+      </c>
+      <c r="C28" s="52">
+        <v>4.6280597E-2</v>
+      </c>
+      <c r="D28" s="52">
+        <v>8.0331610000000005E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="52">
+        <v>2.3017378150000001</v>
+      </c>
+      <c r="C29" s="52">
+        <v>4.9745450000000004E-3</v>
+      </c>
+      <c r="D29" s="52">
+        <v>2.9600000000000001E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="52">
+        <v>2.412437283</v>
+      </c>
+      <c r="C30" s="52">
+        <v>2.0266669999999998E-3</v>
+      </c>
+      <c r="D30" s="52">
+        <v>2.7794289999999999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="52">
+        <v>2.450771188</v>
+      </c>
+      <c r="C31" s="52">
+        <v>1.4862222E-2</v>
+      </c>
+      <c r="D31" s="52">
+        <v>5.9607799999999999E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="52">
+        <v>2.7528237230000001</v>
+      </c>
+      <c r="C32" s="52">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="D32" s="52">
+        <v>3.4350279999999902E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="52">
+        <v>3.6359027080000001</v>
+      </c>
+      <c r="C33" s="52">
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="D33" s="52">
+        <v>1.06047E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" s="52">
+        <v>3.6491520450000001</v>
+      </c>
+      <c r="C34" s="52">
+        <v>2.1699999999999999E-5</v>
+      </c>
+      <c r="D34" s="52">
+        <v>8.3669699999999996E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="52">
+        <v>4.6721431469999999</v>
+      </c>
+      <c r="C35" s="52">
+        <v>1.105455E-3</v>
+      </c>
+      <c r="D35" s="52">
+        <v>2.7866667000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" s="52">
+        <v>5.1795654779999998</v>
+      </c>
+      <c r="C36" s="52">
+        <v>2.1699999999999999E-5</v>
+      </c>
+      <c r="D36" s="52">
+        <v>9.6500000000000008E-6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="52">
+        <v>5.8545579510000003</v>
+      </c>
+      <c r="C37" s="52">
+        <v>3.3295237999999998E-2</v>
+      </c>
+      <c r="D37" s="52">
+        <v>1.5092199999999999E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" s="52">
+        <v>6.6802569910000003</v>
+      </c>
+      <c r="C38" s="52">
+        <v>2.1714289999999999E-3</v>
+      </c>
+      <c r="D38" s="52">
+        <v>5.9607799999999999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" s="52">
+        <v>7.9730357710000002</v>
+      </c>
+      <c r="C39" s="52">
+        <v>2.1699999999999999E-5</v>
+      </c>
+      <c r="D39" s="52">
+        <v>8.3669699999999996E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" s="52">
+        <v>8.5781593770000004</v>
+      </c>
+      <c r="C40" s="52">
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="D40" s="52">
+        <v>8.3669699999999996E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="52">
+        <v>9.5436579649999995</v>
+      </c>
+      <c r="C41" s="52">
+        <v>2.1699999999999999E-5</v>
+      </c>
+      <c r="D41" s="52">
+        <v>7.5099999999999901E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="52">
+        <v>10.3654771999999</v>
+      </c>
+      <c r="C42" s="52">
+        <v>6.2358969999999998E-3</v>
+      </c>
+      <c r="D42" s="52">
+        <v>3.5956999999999997E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" s="52">
+        <v>10.878546869999999</v>
+      </c>
+      <c r="C43" s="52">
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="D43" s="52">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="B44" s="52">
+        <v>14.58758271</v>
+      </c>
+      <c r="C44" s="52">
+        <v>2.1699999999999999E-5</v>
+      </c>
+      <c r="D44" s="52">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" s="52">
+        <v>14.771814940000001</v>
+      </c>
+      <c r="C45" s="52">
+        <v>2.7083636000000001E-2</v>
+      </c>
+      <c r="D45" s="52">
+        <v>3.3043500000000002E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="52">
+        <v>15.80675986</v>
+      </c>
+      <c r="C46" s="52">
+        <v>2.1714289999999999E-3</v>
+      </c>
+      <c r="D46" s="52">
+        <v>9.6500000000000008E-6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47" s="52">
+        <v>44.590952729999998</v>
+      </c>
+      <c r="C47" s="52">
+        <v>6.0799999999999899E-3</v>
+      </c>
+      <c r="D47" s="52">
+        <v>4.5098899999999999E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="B48" s="52">
+        <v>51.603917869999997</v>
+      </c>
+      <c r="C48" s="52">
+        <v>2.1699999999999999E-5</v>
+      </c>
+      <c r="D48" s="52">
+        <v>5.8499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="B49" s="52">
+        <v>88.215004789999995</v>
+      </c>
+      <c r="C49" s="52">
+        <v>4.2375757999999999E-2</v>
+      </c>
+      <c r="D49" s="52">
+        <v>4.1988950000000002E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>